<commit_message>
update leaf mass and area
</commit_message>
<xml_diff>
--- a/data/Croissance_feuille_C3M42.xlsx
+++ b/data/Croissance_feuille_C3M42.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis/Documents/Encadrements/Stages/2021 - M2 - Benoit Berthet - Endopolyploidy/R_Git_PLASTENDO/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8859F71A-3171-4142-8CF3-2AF09015E876}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E227C8-0A20-9745-B90A-95F6430C80BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10580" yWindow="3280" windowWidth="31740" windowHeight="18820" xr2:uid="{3577ABC1-5DAF-441F-9402-2875EC78EF87}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{3577ABC1-5DAF-441F-9402-2875EC78EF87}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="12" r:id="rId1"/>

</xml_diff>